<commit_message>
Multiples mejoras en la interfaz de creacion a nivel programador
</commit_message>
<xml_diff>
--- a/Info Personajes.xlsx
+++ b/Info Personajes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Vida</t>
   </si>
@@ -93,15 +93,6 @@
     <t>Precio Madera</t>
   </si>
   <si>
-    <t>80+30</t>
-  </si>
-  <si>
-    <t>60+20</t>
-  </si>
-  <si>
-    <t>40+20</t>
-  </si>
-  <si>
     <t>Numero max</t>
   </si>
   <si>
@@ -133,12 +124,6 @@
   </si>
   <si>
     <t>Ataque/ segundo</t>
-  </si>
-  <si>
-    <t>2500+100%</t>
-  </si>
-  <si>
-    <t>1000+75%</t>
   </si>
   <si>
     <t>200+35%</t>
@@ -260,13 +245,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +549,7 @@
   <dimension ref="A2:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -585,35 +570,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="A2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="A2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
       <c r="K3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -622,13 +607,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>1</v>
@@ -649,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>3</v>
@@ -666,16 +651,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <f>200*(1+0.2*($K$3-1))</f>
-        <v>200</v>
+        <f>200*$K$3</f>
+        <v>600</v>
       </c>
       <c r="C5">
         <f>100+0.15*($K$3-1)*100</f>
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D5">
         <f>C5*E5</f>
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -688,7 +673,7 @@
       </c>
       <c r="H5">
         <f>3*(1+0.05*($K$3-1))</f>
-        <v>3</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="I5" s="10">
         <v>6</v>
@@ -699,7 +684,7 @@
       </c>
       <c r="L5">
         <f>40*(1+0.5*($K$3-1))</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="M5" s="6">
         <v>5</v>
@@ -707,7 +692,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="4"/>
       <c r="P5" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -716,15 +701,15 @@
       </c>
       <c r="B6">
         <f>150*(1+0.2*($K$3-1))</f>
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="C6">
         <f>200+0.125*($K$3-1)*200</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D9" si="0">C6*E6</f>
-        <v>150</v>
+        <v>187.5</v>
       </c>
       <c r="E6">
         <v>0.75</v>
@@ -737,7 +722,7 @@
       </c>
       <c r="H6">
         <f>3*(1+0.02*($K$3-1))</f>
-        <v>3</v>
+        <v>3.12</v>
       </c>
       <c r="I6" s="10">
         <v>6</v>
@@ -749,8 +734,8 @@
         <v>4</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L6:L9" si="1">40*(1+0.5*($K$3-1))</f>
-        <v>40</v>
+        <f t="shared" ref="L6" si="1">40*(1+0.5*($K$3-1))</f>
+        <v>80</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
@@ -758,7 +743,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="4"/>
       <c r="P6" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -767,15 +752,15 @@
       </c>
       <c r="B7">
         <f>250*(1+0.15*($K$3-1))</f>
-        <v>250</v>
+        <v>325</v>
       </c>
       <c r="C7">
         <f>200+0.15*($K$3-1)*200</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>390</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -788,7 +773,7 @@
       </c>
       <c r="H7">
         <f>10*(1+0.1*($K$3-1))</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I7" s="10">
         <v>8</v>
@@ -801,7 +786,7 @@
       </c>
       <c r="L7">
         <f>50*(1+0.5*($K$3-1))</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M7" s="6">
         <v>6</v>
@@ -809,7 +794,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="4"/>
       <c r="P7" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -818,15 +803,15 @@
       </c>
       <c r="B8">
         <f>300*(1+0.25*($K$3-1))</f>
-        <v>300</v>
+        <v>450</v>
       </c>
       <c r="C8">
         <f>200+0.175*($K$3-1)*200</f>
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>405</v>
       </c>
       <c r="E8">
         <v>1.5</v>
@@ -839,7 +824,7 @@
       </c>
       <c r="H8">
         <f>4.5*(1+0.15*($K$3-1))</f>
-        <v>4.5</v>
+        <v>5.8500000000000005</v>
       </c>
       <c r="I8" s="10">
         <v>7</v>
@@ -852,7 +837,7 @@
       </c>
       <c r="L8">
         <f>100*(1+0.5*($K$3-1))</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M8" s="6">
         <v>7</v>
@@ -860,7 +845,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
       <c r="P8" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -869,15 +854,15 @@
       </c>
       <c r="B9">
         <f>1000*(1+0.3*($K$3-1))</f>
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="C9">
         <f>100+0.25*($K$3-1)*100</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>375</v>
       </c>
       <c r="E9">
         <v>2.5</v>
@@ -890,7 +875,7 @@
       </c>
       <c r="H9">
         <f>3*(1+0.3*($K$3-1))</f>
-        <v>3</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="I9" s="10">
         <v>10</v>
@@ -903,7 +888,7 @@
       </c>
       <c r="L9">
         <f>150*(1+0.5*($K$3-1))</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>15</v>
@@ -911,7 +896,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="4"/>
       <c r="P9" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -926,31 +911,31 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="A13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
       <c r="J14">
         <v>1</v>
       </c>
@@ -970,13 +955,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="H15" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>1</v>
@@ -999,17 +984,19 @@
       <c r="C16" s="10">
         <v>0</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>40</v>
+      <c r="D16" s="10">
+        <f>80+30*($J$14-1)</f>
+        <v>80</v>
+      </c>
+      <c r="E16" s="10">
+        <f>1000*(1+0.75*($J$14-1))</f>
+        <v>1000</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1028,17 +1015,19 @@
       <c r="C17" s="10">
         <v>0</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="10">
+        <f>40+20*($J$14-1)</f>
         <v>40</v>
       </c>
+      <c r="E17" s="10">
+        <f t="shared" ref="E17:E19" si="2">1000*(1+0.75*($J$14-1))</f>
+        <v>1000</v>
+      </c>
       <c r="F17" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1057,17 +1046,19 @@
       <c r="C18" s="10">
         <v>0</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="10">
+        <f>60+40*($J$14-1)</f>
+        <v>60</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="G18" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1086,17 +1077,19 @@
       <c r="C19" s="10">
         <v>0</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="10">
+        <f>40+20*($J$14-1)</f>
+        <v>40</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="G19" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1117,15 +1110,16 @@
       <c r="D20" s="10">
         <v>0</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>39</v>
+      <c r="E20" s="10">
+        <f>2500*(1+2*($J$14-1))</f>
+        <v>2500</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I20" s="10">
         <v>30</v>
@@ -1154,6 +1148,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D18" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cambio en la forma de generar, más optimizado
</commit_message>
<xml_diff>
--- a/Info Personajes.xlsx
+++ b/Info Personajes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="14115" windowHeight="4695"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="9120" windowHeight="4695"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -598,7 +598,7 @@
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -652,15 +652,15 @@
       </c>
       <c r="B5">
         <f>200*$K$3</f>
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <f>100+0.15*($K$3-1)*100</f>
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <f>C5*E5</f>
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -673,7 +673,7 @@
       </c>
       <c r="H5">
         <f>3*(1+0.05*($K$3-1))</f>
-        <v>3.3000000000000003</v>
+        <v>3</v>
       </c>
       <c r="I5" s="10">
         <v>6</v>
@@ -684,7 +684,7 @@
       </c>
       <c r="L5">
         <f>40*(1+0.5*($K$3-1))</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="M5" s="6">
         <v>5</v>
@@ -701,15 +701,15 @@
       </c>
       <c r="B6">
         <f>150*(1+0.2*($K$3-1))</f>
-        <v>210</v>
+        <v>150</v>
       </c>
       <c r="C6">
         <f>200+0.125*($K$3-1)*200</f>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D9" si="0">C6*E6</f>
-        <v>187.5</v>
+        <v>150</v>
       </c>
       <c r="E6">
         <v>0.75</v>
@@ -722,7 +722,7 @@
       </c>
       <c r="H6">
         <f>3*(1+0.02*($K$3-1))</f>
-        <v>3.12</v>
+        <v>3</v>
       </c>
       <c r="I6" s="10">
         <v>6</v>
@@ -735,7 +735,7 @@
       </c>
       <c r="L6">
         <f t="shared" ref="L6" si="1">40*(1+0.5*($K$3-1))</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="M6" s="6">
         <v>2</v>
@@ -752,15 +752,15 @@
       </c>
       <c r="B7">
         <f>250*(1+0.15*($K$3-1))</f>
-        <v>325</v>
+        <v>250</v>
       </c>
       <c r="C7">
         <f>200+0.15*($K$3-1)*200</f>
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -773,7 +773,7 @@
       </c>
       <c r="H7">
         <f>10*(1+0.1*($K$3-1))</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I7" s="10">
         <v>8</v>
@@ -786,7 +786,7 @@
       </c>
       <c r="L7">
         <f>50*(1+0.5*($K$3-1))</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M7" s="6">
         <v>6</v>
@@ -803,15 +803,15 @@
       </c>
       <c r="B8">
         <f>300*(1+0.25*($K$3-1))</f>
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="C8">
         <f>200+0.175*($K$3-1)*200</f>
-        <v>270</v>
+        <v>200</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>405</v>
+        <v>300</v>
       </c>
       <c r="E8">
         <v>1.5</v>
@@ -824,7 +824,7 @@
       </c>
       <c r="H8">
         <f>4.5*(1+0.15*($K$3-1))</f>
-        <v>5.8500000000000005</v>
+        <v>4.5</v>
       </c>
       <c r="I8" s="10">
         <v>7</v>
@@ -837,7 +837,7 @@
       </c>
       <c r="L8">
         <f>100*(1+0.5*($K$3-1))</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M8" s="6">
         <v>7</v>
@@ -854,15 +854,15 @@
       </c>
       <c r="B9">
         <f>1000*(1+0.3*($K$3-1))</f>
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="C9">
         <f>100+0.25*($K$3-1)*100</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>375</v>
+        <v>250</v>
       </c>
       <c r="E9">
         <v>2.5</v>
@@ -875,7 +875,7 @@
       </c>
       <c r="H9">
         <f>3*(1+0.3*($K$3-1))</f>
-        <v>4.8000000000000007</v>
+        <v>3</v>
       </c>
       <c r="I9" s="10">
         <v>10</v>
@@ -888,7 +888,7 @@
       </c>
       <c r="L9">
         <f>150*(1+0.5*($K$3-1))</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>15</v>

</xml_diff>